<commit_message>
pressure agnostic model fitting exploration
</commit_message>
<xml_diff>
--- a/PIECM/data/ECM_Params.xlsx
+++ b/PIECM/data/ECM_Params.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KatieLukow/Documents/git-repos/fitted_ECM/PIECM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F946CA-C2AB-B14D-8DFC-CD1F5C6B7953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711ED622-84D4-BB47-90E9-CCDFA6271F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="20320" xr2:uid="{35A3DEA1-7664-804A-B334-72214D1BA623}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -116,10 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCA0581-7F5D-3846-8282-4DEE9F1FBD26}">
   <dimension ref="A3:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,15 +645,15 @@
       <c r="K21" s="1">
         <v>0.1722071</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21">
         <f>AVERAGE(B21:K21)</f>
         <v>0.26807723</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21">
         <f>MAX(B21:K21)</f>
         <v>0.37661159999999999</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21">
         <f>MIN(B21:K21)</f>
         <v>0.1722071</v>
       </c>
@@ -693,9 +692,6 @@
       <c r="K22">
         <v>-35.835583461640603</v>
       </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -731,9 +727,6 @@
       <c r="K23">
         <v>1.4914627620544999E-4</v>
       </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -769,9 +762,6 @@
       <c r="K24">
         <v>35.839491186569298</v>
       </c>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -807,9 +797,6 @@
       <c r="K25">
         <v>119291.28045585399</v>
       </c>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -845,9 +832,6 @@
       <c r="K26">
         <v>67262.274301520694</v>
       </c>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -883,9 +867,6 @@
       <c r="K27">
         <v>2.2032453204271998</v>
       </c>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -921,9 +902,6 @@
       <c r="K28">
         <v>1.01052653545809E-2</v>
       </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -932,22 +910,15 @@
       <c r="D29">
         <v>0.2765993452544</v>
       </c>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="L29">
+        <f>AVERAGE(L21,L33,L45)</f>
+        <v>0.27221684333333335</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B32">
@@ -980,9 +951,6 @@
       <c r="K32">
         <v>10</v>
       </c>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1018,15 +986,15 @@
       <c r="K33" s="1">
         <v>0.21379790000000001</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33">
         <f>AVERAGE(B33:K33)</f>
         <v>0.31077112999999995</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33">
         <f>MAX(B33:K33)</f>
         <v>0.4186954</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33">
         <f>MIN(B33:K33)</f>
         <v>0.21379790000000001</v>
       </c>
@@ -1065,9 +1033,6 @@
       <c r="K34">
         <v>0.22953534803459</v>
       </c>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1103,9 +1068,6 @@
       <c r="K35">
         <v>11.7837843954429</v>
       </c>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1141,9 +1103,6 @@
       <c r="K36">
         <v>-12.008943961588701</v>
       </c>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1179,9 +1138,6 @@
       <c r="K37">
         <v>42.582744706816001</v>
       </c>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1217,9 +1173,6 @@
       <c r="K38">
         <v>6.5385434338012898</v>
       </c>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1255,9 +1208,10 @@
       <c r="K39">
         <v>343364.19825392897</v>
       </c>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+      <c r="L39">
+        <f>L33/L41</f>
+        <v>0.30802105509982713</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -1293,9 +1247,6 @@
       <c r="K40">
         <v>1.10809451535323E-2</v>
       </c>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1331,31 +1282,23 @@
       <c r="K41">
         <v>0.80341528501364201</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41">
         <f>AVERAGE(B41:K41)</f>
         <v>1.0089282042725343</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M41">
         <f>MAX(B41:K41)</f>
         <v>1.56732433504212</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N41">
         <f>MIN(B41:K41)</f>
         <v>0.79456347034727903</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B44">
@@ -1388,9 +1331,6 @@
       <c r="K44">
         <v>10</v>
       </c>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -1426,15 +1366,15 @@
       <c r="K45" s="1">
         <v>0.1282431</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L45">
         <f>AVERAGE(B45:K45)</f>
         <v>0.23780217000000001</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45">
         <f>MAX(B45:K45)</f>
         <v>0.37445309999999998</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45">
         <f>MIN(B45:K45)</f>
         <v>0.1282431</v>
       </c>

</xml_diff>

<commit_message>
fix date-time in data
</commit_message>
<xml_diff>
--- a/PIECM/data/ECM_Params.xlsx
+++ b/PIECM/data/ECM_Params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KatieLukow/Documents/git-repos/fitted_ECM/PIECM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711ED622-84D4-BB47-90E9-CCDFA6271F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933BD349-DCB2-C549-8922-AF4C727F0AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="20320" xr2:uid="{35A3DEA1-7664-804A-B334-72214D1BA623}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>R1</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>1RC</t>
+  </si>
+  <si>
+    <t>2RC</t>
+  </si>
+  <si>
+    <t>3RC</t>
   </si>
 </sst>
 </file>
@@ -433,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCA0581-7F5D-3846-8282-4DEE9F1FBD26}">
-  <dimension ref="A3:N52"/>
+  <dimension ref="A3:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,7 +1493,7 @@
         <v>1.48034547730522</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>8.9013134860241099</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1554,7 +1563,7 @@
         <v>120174.674005678</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1589,7 +1598,7 @@
         <v>5.7302483993680502</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1622,6 +1631,173 @@
       </c>
       <c r="K52">
         <v>9.8504614285636199E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L53">
+        <f>AVERAGE(L21,L33,L45,)</f>
+        <v>0.2041626325</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>100</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.47239999999999999</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.47003719999999999</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.29702319999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>90</v>
+      </c>
+      <c r="B58">
+        <v>0.38482</v>
+      </c>
+      <c r="C58">
+        <v>0.45051999999999998</v>
+      </c>
+      <c r="D58">
+        <v>0.25930999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>80</v>
+      </c>
+      <c r="B59">
+        <v>0.39062999999999998</v>
+      </c>
+      <c r="C59">
+        <v>0.48894700000000002</v>
+      </c>
+      <c r="D59">
+        <v>0.2723777</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>70</v>
+      </c>
+      <c r="B60">
+        <v>0.40162999999999999</v>
+      </c>
+      <c r="C60">
+        <v>0.490838</v>
+      </c>
+      <c r="D60">
+        <v>0.29239599999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>0.40132200000000001</v>
+      </c>
+      <c r="C61">
+        <v>0.48226799999999997</v>
+      </c>
+      <c r="D61">
+        <v>0.30452000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>50</v>
+      </c>
+      <c r="B62">
+        <v>0.38605099999999998</v>
+      </c>
+      <c r="C62">
+        <v>0.48337000000000002</v>
+      </c>
+      <c r="D62">
+        <v>0.28462799999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>40</v>
+      </c>
+      <c r="B63">
+        <v>0.41930800000000001</v>
+      </c>
+      <c r="C63">
+        <v>0.57841480000000001</v>
+      </c>
+      <c r="D63">
+        <v>0.36316599999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>30</v>
+      </c>
+      <c r="B64">
+        <v>0.4473008</v>
+      </c>
+      <c r="C64">
+        <v>0.66423299999999996</v>
+      </c>
+      <c r="D64">
+        <v>0.41869469999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>20</v>
+      </c>
+      <c r="B65">
+        <v>0.43763000000000002</v>
+      </c>
+      <c r="C65">
+        <v>0.57943960000000005</v>
+      </c>
+      <c r="D65">
+        <v>0.40178950000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>0.38205040000000001</v>
+      </c>
+      <c r="C66">
+        <v>0.21379100000000001</v>
+      </c>
+      <c r="D66">
+        <v>0.21379000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="1">
+        <f>AVERAGE(B57:B66)</f>
+        <v>0.41231422000000001</v>
+      </c>
+      <c r="D68" s="1">
+        <f>AVERAGE(D57:D66)</f>
+        <v>0.31076951000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
python + julia fixes
</commit_message>
<xml_diff>
--- a/PIECM/data/ECM_Params.xlsx
+++ b/PIECM/data/ECM_Params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katielukow/Documents/git-repos/PressureFitted_ECM/PIECM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C32B976-D6A5-574E-9D4C-677F96C2AC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549CCBED-966E-FC40-A8A8-78E60876E234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="-19980" windowWidth="14400" windowHeight="16100" activeTab="1" xr2:uid="{35A3DEA1-7664-804A-B334-72214D1BA623}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15980" activeTab="1" xr2:uid="{35A3DEA1-7664-804A-B334-72214D1BA623}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
   <si>
     <t>R1</t>
   </si>
@@ -116,12 +116,19 @@
   <si>
     <t>2rc</t>
   </si>
+  <si>
+    <t>bad pressure fitting</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,8 +136,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,8 +165,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,11 +180,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -164,9 +208,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1843,14 +1895,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A2237-5B84-F146-A072-74BEF976396E}">
-  <dimension ref="B3:P55"/>
+  <dimension ref="B3:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="J19" zoomScale="65" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2165,7 +2218,7 @@
         <v>-99.392782077269985</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G17">
         <f>100-ABS(G16)</f>
         <v>0.6072179227300154</v>
@@ -2175,12 +2228,56 @@
         <v>0.13509999999999994</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="K22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="K23" s="7">
+        <v>40</v>
+      </c>
+      <c r="P23" s="7">
+        <v>25</v>
+      </c>
+      <c r="U23" s="7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K24" s="8"/>
+      <c r="L24" s="9">
+        <v>40</v>
+      </c>
+      <c r="M24" s="8">
+        <v>25</v>
+      </c>
+      <c r="N24" s="8">
+        <v>130</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>40</v>
+      </c>
+      <c r="R24" s="9">
+        <v>25</v>
+      </c>
+      <c r="S24" s="8">
+        <v>130</v>
+      </c>
+      <c r="V24" s="8">
+        <v>40</v>
+      </c>
+      <c r="W24" s="10">
+        <v>25</v>
+      </c>
+      <c r="X24" s="9">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>18</v>
       </c>
@@ -2199,21 +2296,57 @@
       <c r="H25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K25" s="8">
+        <v>100</v>
+      </c>
+      <c r="L25" s="9">
+        <v>1.20514085797111E-2</v>
+      </c>
+      <c r="M25" s="8">
+        <v>1.9713030785961299E-2</v>
+      </c>
+      <c r="N25" s="8">
+        <v>2.1029734328836699E-2</v>
+      </c>
+      <c r="P25">
+        <v>100</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>1.59337906151986E-2</v>
+      </c>
+      <c r="R25" s="9">
+        <v>1.0553681203737101E-2</v>
+      </c>
+      <c r="S25" s="8">
+        <v>1.01890979711316E-2</v>
+      </c>
+      <c r="U25">
+        <v>100</v>
+      </c>
+      <c r="V25" s="8">
+        <v>1.8633937966488899E-2</v>
+      </c>
+      <c r="W25" s="10">
+        <v>1.1671043011221301E-2</v>
+      </c>
+      <c r="X25" s="9">
+        <v>8.4746770776052693E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>100</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="5">
         <v>123.36499999999999</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>1.8482066102096901E-3</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="5">
         <v>106.42700000000001</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="6">
         <v>1.8482099486615501E-3</v>
       </c>
       <c r="G26">
@@ -2224,21 +2357,57 @@
         <f>C26-E26</f>
         <v>16.937999999999988</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K26" s="8">
+        <v>90</v>
+      </c>
+      <c r="L26" s="9">
+        <v>1.38047882636651E-2</v>
+      </c>
+      <c r="M26" s="8">
+        <v>2.18504498144521E-2</v>
+      </c>
+      <c r="N26" s="8">
+        <v>2.5072392735572401E-2</v>
+      </c>
+      <c r="P26">
+        <v>90</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>2.2670969303926699E-2</v>
+      </c>
+      <c r="R26" s="9">
+        <v>1.27019995049117E-2</v>
+      </c>
+      <c r="S26" s="8">
+        <v>1.3624210229426699E-2</v>
+      </c>
+      <c r="U26">
+        <v>90</v>
+      </c>
+      <c r="V26" s="8">
+        <v>2.58659124799E-2</v>
+      </c>
+      <c r="W26" s="10">
+        <v>1.37625873167617E-2</v>
+      </c>
+      <c r="X26" s="9">
+        <v>1.2634663932254301E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>90</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="5">
         <v>108.143</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>4.8734322265080697E-3</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="5">
         <v>91.256</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="6">
         <v>4.8734342518153197E-3</v>
       </c>
       <c r="G27">
@@ -2249,21 +2418,57 @@
         <f>C27-E27</f>
         <v>16.887</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K27" s="8">
+        <v>80</v>
+      </c>
+      <c r="L27" s="9">
+        <v>1.41096701366989E-2</v>
+      </c>
+      <c r="M27" s="8">
+        <v>2.2288955715876801E-2</v>
+      </c>
+      <c r="N27" s="8">
+        <v>2.47730237027417E-2</v>
+      </c>
+      <c r="P27">
+        <v>80</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>2.31406506107983E-2</v>
+      </c>
+      <c r="R27" s="9">
+        <v>1.2723955854867E-2</v>
+      </c>
+      <c r="S27" s="8">
+        <v>1.2884792524791199E-2</v>
+      </c>
+      <c r="U27">
+        <v>80</v>
+      </c>
+      <c r="V27" s="8">
+        <v>2.5644508925281102E-2</v>
+      </c>
+      <c r="W27" s="10">
+        <v>1.3097780203017099E-2</v>
+      </c>
+      <c r="X27" s="9">
+        <v>1.25030175442527E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>80</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>109.63</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>6.74321854155402E-3</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="5">
         <v>93.792000000000002</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="6">
         <v>6.7432238681517697E-3</v>
       </c>
       <c r="G28">
@@ -2274,21 +2479,57 @@
         <f>C28-E28</f>
         <v>15.837999999999994</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K28" s="8">
+        <v>70</v>
+      </c>
+      <c r="L28" s="9">
+        <v>1.32266543475794E-2</v>
+      </c>
+      <c r="M28" s="8">
+        <v>2.2670899157301E-2</v>
+      </c>
+      <c r="N28" s="8">
+        <v>2.5615629651356601E-2</v>
+      </c>
+      <c r="P28">
+        <v>70</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>2.3583449079185199E-2</v>
+      </c>
+      <c r="R28" s="9">
+        <v>1.1491399824413899E-2</v>
+      </c>
+      <c r="S28" s="8">
+        <v>1.2099811767114501E-2</v>
+      </c>
+      <c r="U28">
+        <v>70</v>
+      </c>
+      <c r="V28" s="8">
+        <v>2.6560441229832199E-2</v>
+      </c>
+      <c r="W28" s="10">
+        <v>1.2345561977964501E-2</v>
+      </c>
+      <c r="X28" s="9">
+        <v>1.12878727291667E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>70</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="5">
         <v>107.524</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>8.2324176714451101E-3</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="5">
         <v>91.650999999999996</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="6">
         <v>8.2324211937105998E-3</v>
       </c>
       <c r="G29">
@@ -2299,21 +2540,57 @@
         <f>C29-E29</f>
         <v>15.873000000000005</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K29" s="8">
+        <v>60</v>
+      </c>
+      <c r="L29" s="9">
+        <v>1.21836701340103E-2</v>
+      </c>
+      <c r="M29" s="8">
+        <v>2.81357804840691E-2</v>
+      </c>
+      <c r="N29" s="8">
+        <v>3.06671418001358E-2</v>
+      </c>
+      <c r="P29">
+        <v>60</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>2.7159823411525501E-2</v>
+      </c>
+      <c r="R29" s="9">
+        <v>1.08553110727237E-2</v>
+      </c>
+      <c r="S29" s="8">
+        <v>1.12826347218051E-2</v>
+      </c>
+      <c r="U29">
+        <v>60</v>
+      </c>
+      <c r="V29" s="8">
+        <v>2.9995952555619199E-2</v>
+      </c>
+      <c r="W29" s="10">
+        <v>1.16594659287716E-2</v>
+      </c>
+      <c r="X29" s="9">
+        <v>1.0454981990813499E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>60</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="5">
         <v>115.658</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>6.12830880190934E-3</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="5">
         <v>97.551000000000002</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="6">
         <v>6.1283105814866198E-3</v>
       </c>
       <c r="G30">
@@ -2324,21 +2601,57 @@
         <f>C30-E30</f>
         <v>18.106999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K30" s="8">
+        <v>50</v>
+      </c>
+      <c r="L30" s="9">
+        <v>1.2659332468500199E-2</v>
+      </c>
+      <c r="M30" s="8">
+        <v>2.43902848924837E-2</v>
+      </c>
+      <c r="N30" s="8">
+        <v>2.8697577737195799E-2</v>
+      </c>
+      <c r="P30">
+        <v>50</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>2.4963191054986698E-2</v>
+      </c>
+      <c r="R30" s="9">
+        <v>1.14578105002599E-2</v>
+      </c>
+      <c r="S30" s="8">
+        <v>1.24232275944178E-2</v>
+      </c>
+      <c r="U30">
+        <v>50</v>
+      </c>
+      <c r="V30" s="8">
+        <v>2.9406206765896E-2</v>
+      </c>
+      <c r="W30" s="10">
+        <v>1.2896854003193301E-2</v>
+      </c>
+      <c r="X30" s="9">
+        <v>1.09311099701503E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>50</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>122.533</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>5.6433811165398102E-3</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="5">
         <v>104.126</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="6">
         <v>5.6433841006573301E-3</v>
       </c>
       <c r="G31">
@@ -2349,21 +2662,57 @@
         <f>C31-E31</f>
         <v>18.406999999999996</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K31" s="8">
+        <v>40</v>
+      </c>
+      <c r="L31" s="9">
+        <v>1.2669031947247E-2</v>
+      </c>
+      <c r="M31" s="8">
+        <v>2.7015616999305998E-2</v>
+      </c>
+      <c r="N31" s="8">
+        <v>3.1912495734792698E-2</v>
+      </c>
+      <c r="P31">
+        <v>40</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>2.78957473928436E-2</v>
+      </c>
+      <c r="R31" s="9">
+        <v>1.05665027969922E-2</v>
+      </c>
+      <c r="S31" s="8">
+        <v>1.1651708213939699E-2</v>
+      </c>
+      <c r="U31">
+        <v>40</v>
+      </c>
+      <c r="V31" s="8">
+        <v>3.2836644913086098E-2</v>
+      </c>
+      <c r="W31" s="10">
+        <v>1.2134285220434299E-2</v>
+      </c>
+      <c r="X31" s="9">
+        <v>9.9995181911557707E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>40</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="5">
         <v>115.13</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>7.3817190784420403E-3</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="5">
         <v>98.171000000000006</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="6">
         <v>7.3817209430624897E-3</v>
       </c>
       <c r="G32">
@@ -2374,21 +2723,57 @@
         <f>C32-E32</f>
         <v>16.958999999999989</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="8">
+        <v>30</v>
+      </c>
+      <c r="L32" s="9">
+        <v>1.2322098552017401E-2</v>
+      </c>
+      <c r="M32" s="8">
+        <v>3.2331230151346597E-2</v>
+      </c>
+      <c r="N32" s="8">
+        <v>3.76096003823033E-2</v>
+      </c>
+      <c r="P32">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>3.3268453395697603E-2</v>
+      </c>
+      <c r="R32" s="9">
+        <v>9.5058096120956594E-3</v>
+      </c>
+      <c r="S32" s="8">
+        <v>1.0637769853062799E-2</v>
+      </c>
+      <c r="U32">
+        <v>30</v>
+      </c>
+      <c r="V32" s="8">
+        <v>3.86100939532808E-2</v>
+      </c>
+      <c r="W32" s="10">
+        <v>1.13545033801898E-2</v>
+      </c>
+      <c r="X32" s="9">
+        <v>8.6455719579430195E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>30</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>107.619</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="6">
         <v>8.20006331598944E-3</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="5">
         <v>94.647999999999996</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="6">
         <v>8.2000667283049604E-3</v>
       </c>
       <c r="G33">
@@ -2399,21 +2784,57 @@
         <f>C33-E33</f>
         <v>12.971000000000004</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="8">
+        <v>20</v>
+      </c>
+      <c r="L33" s="9">
+        <v>1.21388050928897E-2</v>
+      </c>
+      <c r="M33" s="8">
+        <v>3.8881886196302902E-2</v>
+      </c>
+      <c r="N33" s="8">
+        <v>4.3895324928647297E-2</v>
+      </c>
+      <c r="P33">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>3.9535037684098197E-2</v>
+      </c>
+      <c r="R33" s="9">
+        <v>9.8111812025060904E-3</v>
+      </c>
+      <c r="S33" s="8">
+        <v>1.0399570112649701E-2</v>
+      </c>
+      <c r="U33">
+        <v>20</v>
+      </c>
+      <c r="V33" s="8">
+        <v>4.47882721157234E-2</v>
+      </c>
+      <c r="W33" s="10">
+        <v>1.1687134651321599E-2</v>
+      </c>
+      <c r="X33" s="9">
+        <v>8.2208183093990302E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>20</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>120.7</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="6">
         <v>7.08656620464314E-3</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="5">
         <v>104.788</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="6">
         <v>7.08657574276725E-3</v>
       </c>
       <c r="G34">
@@ -2424,21 +2845,57 @@
         <f>C34-E34</f>
         <v>15.912000000000006</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="8">
+        <v>10</v>
+      </c>
+      <c r="L34" s="9">
+        <v>1.34770395067458E-2</v>
+      </c>
+      <c r="M34" s="8">
+        <v>4.3988460679129898E-2</v>
+      </c>
+      <c r="N34" s="8">
+        <v>4.93164375612654E-2</v>
+      </c>
+      <c r="P34">
+        <v>10</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>4.5197875733679199E-2</v>
+      </c>
+      <c r="R34" s="9">
+        <v>1.2071505455972799E-2</v>
+      </c>
+      <c r="S34" s="8">
+        <v>1.30987175647654E-2</v>
+      </c>
+      <c r="U34">
+        <v>10</v>
+      </c>
+      <c r="V34" s="8">
+        <v>5.0598526281017998E-2</v>
+      </c>
+      <c r="W34" s="10">
+        <v>1.3763290368036E-2</v>
+      </c>
+      <c r="X34" s="9">
+        <v>1.0485294217328901E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>10</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>85.790999999999997</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="6">
         <v>4.5773208474859601E-3</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="5">
         <v>74.596999999999994</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="6">
         <v>4.57732472301351E-3</v>
       </c>
       <c r="G35">
@@ -2449,14 +2906,79 @@
         <f>C35-E35</f>
         <v>11.194000000000003</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <f>AVERAGE(L25:L34)</f>
+        <v>1.286424990290649E-2</v>
+      </c>
+      <c r="M35">
+        <f t="shared" ref="M35" si="3">AVERAGE(M25:M34)</f>
+        <v>2.812665948762294E-2</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ref="N35" si="4">AVERAGE(N25:N34)</f>
+        <v>3.185893585628477E-2</v>
+      </c>
+      <c r="Q35">
+        <f>AVERAGE(Q25:Q34)</f>
+        <v>2.8334898828193962E-2</v>
+      </c>
+      <c r="R35">
+        <f t="shared" ref="R35" si="5">AVERAGE(R25:R34)</f>
+        <v>1.1173915702848003E-2</v>
+      </c>
+      <c r="S35">
+        <f t="shared" ref="S35" si="6">AVERAGE(S25:S34)</f>
+        <v>1.182915405531045E-2</v>
+      </c>
+      <c r="V35">
+        <f>AVERAGE(V25:V34)</f>
+        <v>3.2294049718612571E-2</v>
+      </c>
+      <c r="W35">
+        <f t="shared" ref="W35:X35" si="7">AVERAGE(W25:W34)</f>
+        <v>1.243725060609112E-2</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="7"/>
+        <v>1.0363752592006949E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G36">
         <f>AVERAGE(G26:G35)</f>
         <v>7.1201913700173097E-5</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="M36" s="11">
+        <f>(M35-L35)/M35</f>
+        <v>0.54263143447349771</v>
+      </c>
+      <c r="N36" s="11">
+        <f>(N35-L35)/N35</f>
+        <v>0.5962121911121907</v>
+      </c>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11">
+        <f>(Q35-R35)/Q35</f>
+        <v>0.60564829362546857</v>
+      </c>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11">
+        <f>(S35-R35)/S35</f>
+        <v>5.5391818332798833E-2</v>
+      </c>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11">
+        <f>(V35-X35)/V35</f>
+        <v>0.6790816672944604</v>
+      </c>
+      <c r="W36" s="11">
+        <f>(W35-X35)/W35</f>
+        <v>0.1667167511337819</v>
+      </c>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E37">
         <f>AVERAGE(E26:E35)</f>
         <v>95.700700000000012</v>
@@ -2470,18 +2992,56 @@
         <v>15.908599999999996</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E38">
         <f>H37/E37</f>
         <v>0.16623284887153381</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="K40" s="7">
+        <v>0</v>
+      </c>
+      <c r="P40" s="7">
+        <v>50</v>
+      </c>
+      <c r="U40" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C41">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L41" s="9">
+        <v>0</v>
+      </c>
+      <c r="M41" s="8">
+        <v>50</v>
+      </c>
+      <c r="N41" s="8">
+        <v>100</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>0</v>
+      </c>
+      <c r="R41" s="9">
+        <v>50</v>
+      </c>
+      <c r="S41" s="8">
+        <v>100</v>
+      </c>
+      <c r="V41" s="8">
+        <v>0</v>
+      </c>
+      <c r="W41" s="8">
+        <v>50</v>
+      </c>
+      <c r="X41" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>18</v>
       </c>
@@ -2500,21 +3060,57 @@
       <c r="H42" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>100</v>
+      </c>
+      <c r="L42" s="9">
+        <v>3.6042557358412302E-3</v>
+      </c>
+      <c r="M42" s="8">
+        <v>6.0168176869929597E-3</v>
+      </c>
+      <c r="N42" s="8">
+        <v>8.7981339510285004E-3</v>
+      </c>
+      <c r="P42">
+        <v>100</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>5.33802945454103E-3</v>
+      </c>
+      <c r="R42" s="9">
+        <v>4.57732472301351E-3</v>
+      </c>
+      <c r="S42" s="8">
+        <v>6.6928662190404902E-3</v>
+      </c>
+      <c r="U42">
+        <v>100</v>
+      </c>
+      <c r="V42" s="8">
+        <v>8.1327277709610808E-3</v>
+      </c>
+      <c r="W42" s="8">
+        <v>6.3655580984447102E-3</v>
+      </c>
+      <c r="X42" s="9">
+        <v>5.0175673205011496E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>100</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="5">
         <v>109.746</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="6">
         <v>1.8482120769911399E-3</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="5">
         <v>227.09399999999999</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="6">
         <v>3.6092468767544698E-3</v>
       </c>
       <c r="G43">
@@ -2525,75 +3121,183 @@
         <f>C43-E43</f>
         <v>-117.348</v>
       </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>90</v>
+      </c>
+      <c r="L43" s="9">
+        <v>6.1310102754400702E-3</v>
+      </c>
+      <c r="M43" s="8">
+        <v>7.9869551352521294E-3</v>
+      </c>
+      <c r="N43" s="8">
+        <v>9.4230423392597795E-3</v>
+      </c>
+      <c r="P43">
+        <v>90</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>7.1242398539241502E-3</v>
+      </c>
+      <c r="R43" s="9">
+        <v>7.0865702113395703E-3</v>
+      </c>
+      <c r="S43" s="8">
+        <v>8.4561259597547098E-3</v>
+      </c>
+      <c r="U43">
+        <v>90</v>
+      </c>
+      <c r="V43" s="8">
+        <v>8.5517869904965897E-3</v>
+      </c>
+      <c r="W43" s="8">
+        <v>8.3111890308680495E-3</v>
+      </c>
+      <c r="X43" s="9">
+        <v>7.3007551798421402E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>90</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="5">
         <v>98.156000000000006</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="6">
         <v>4.8734342518153197E-3</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="5">
         <v>188.709</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="6">
         <v>6.3996866180350796E-3</v>
       </c>
       <c r="G44">
-        <f t="shared" ref="G44:G54" si="3">((((F44-D44)/F44)))*100</f>
+        <f t="shared" ref="G44:G54" si="8">((((F44-D44)/F44)))*100</f>
         <v>23.848861003890391</v>
       </c>
       <c r="H44">
         <f>C44-E44</f>
         <v>-90.552999999999997</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <v>80</v>
+      </c>
+      <c r="L44" s="9">
+        <v>8.0483296607342207E-3</v>
+      </c>
+      <c r="M44" s="8">
+        <v>8.4036024040301995E-3</v>
+      </c>
+      <c r="N44" s="8">
+        <v>9.5322741770186604E-3</v>
+      </c>
+      <c r="P44">
+        <v>80</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>8.2427533543529899E-3</v>
+      </c>
+      <c r="R44" s="9">
+        <v>8.2000667283049604E-3</v>
+      </c>
+      <c r="S44" s="8">
+        <v>9.3308233454571701E-3</v>
+      </c>
+      <c r="U44">
+        <v>80</v>
+      </c>
+      <c r="V44" s="8">
+        <v>9.2305382292011493E-3</v>
+      </c>
+      <c r="W44" s="8">
+        <v>9.1653850851593499E-3</v>
+      </c>
+      <c r="X44" s="9">
+        <v>8.3881670010002296E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>80</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="5">
         <v>96.052000000000007</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="6">
         <v>6.7432186711176602E-3</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="5">
         <v>186.25</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="6">
         <v>8.7308604768602197E-3</v>
       </c>
       <c r="G45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>22.765703460850087</v>
       </c>
       <c r="H45">
         <f>C45-E45</f>
         <v>-90.197999999999993</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>70</v>
+      </c>
+      <c r="L45" s="9">
+        <v>7.2324080785703803E-3</v>
+      </c>
+      <c r="M45" s="8">
+        <v>7.4681367064375103E-3</v>
+      </c>
+      <c r="N45" s="8">
+        <v>8.7860224731295695E-3</v>
+      </c>
+      <c r="P45">
+        <v>70</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>7.3139733543262E-3</v>
+      </c>
+      <c r="R45" s="9">
+        <v>7.3817209430624897E-3</v>
+      </c>
+      <c r="S45" s="8">
+        <v>8.7796313240783904E-3</v>
+      </c>
+      <c r="U45">
+        <v>70</v>
+      </c>
+      <c r="V45" s="8">
+        <v>8.4060017337264405E-3</v>
+      </c>
+      <c r="W45" s="8">
+        <v>8.5307761418924408E-3</v>
+      </c>
+      <c r="X45" s="9">
+        <v>7.6651452086227596E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>70</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="5">
         <v>96.04</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="6">
         <v>8.2324211937105998E-3</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="5">
         <v>193.006</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="6">
         <v>1.12317956992713E-2</v>
       </c>
       <c r="G46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>26.704318577974977</v>
       </c>
       <c r="H46">
@@ -2604,169 +3308,463 @@
         <f>F46-D46</f>
         <v>2.9993745055607E-3</v>
       </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>60</v>
+      </c>
+      <c r="L46" s="9">
+        <v>5.2886081405464696E-3</v>
+      </c>
+      <c r="M46" s="8">
+        <v>5.6904363009969098E-3</v>
+      </c>
+      <c r="N46" s="8">
+        <v>7.6975679522066597E-3</v>
+      </c>
+      <c r="P46">
+        <v>60</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>5.3378813137547098E-3</v>
+      </c>
+      <c r="R46" s="9">
+        <v>5.6433841006573301E-3</v>
+      </c>
+      <c r="S46" s="8">
+        <v>7.67367061912708E-3</v>
+      </c>
+      <c r="U46">
+        <v>60</v>
+      </c>
+      <c r="V46" s="8">
+        <v>7.0280008174422298E-3</v>
+      </c>
+      <c r="W46" s="8">
+        <v>7.2647518254569301E-3</v>
+      </c>
+      <c r="X46" s="9">
+        <v>6.1072279224231203E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>60</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="5">
         <v>101.922</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="6">
         <v>6.1283146844481199E-3</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="5">
         <v>204.54300000000001</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="6">
         <v>3.3389006283308098E-3</v>
       </c>
       <c r="G47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>-83.542889310599207</v>
       </c>
       <c r="H47">
         <f>C47-E47</f>
         <v>-102.62100000000001</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>50</v>
+      </c>
+      <c r="L47" s="9">
+        <v>5.1827892207384398E-3</v>
+      </c>
+      <c r="M47" s="8">
+        <v>6.2596898210953997E-3</v>
+      </c>
+      <c r="N47" s="8">
+        <v>7.1060686608948398E-3</v>
+      </c>
+      <c r="P47">
+        <v>50</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>5.3600217914321104E-3</v>
+      </c>
+      <c r="R47" s="9">
+        <v>6.1283146844481199E-3</v>
+      </c>
+      <c r="S47" s="8">
+        <v>6.81076165415138E-3</v>
+      </c>
+      <c r="U47">
+        <v>50</v>
+      </c>
+      <c r="V47" s="8">
+        <v>5.9860507614975696E-3</v>
+      </c>
+      <c r="W47" s="8">
+        <v>6.4779605156337697E-3</v>
+      </c>
+      <c r="X47" s="9">
+        <v>6.4907647953909497E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>50</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="5">
         <v>103.253</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="6">
         <v>5.6433841006573301E-3</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="5">
         <v>175.67099999999999</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="6">
         <v>6.7769888148821698E-3</v>
       </c>
       <c r="G48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>16.727262582099296</v>
       </c>
       <c r="H48">
         <f>C48-E48</f>
         <v>-72.417999999999992</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>40</v>
+      </c>
+      <c r="L48" s="9">
+        <v>8.2167305001251394E-3</v>
+      </c>
+      <c r="M48" s="8">
+        <v>8.4436811660434201E-3</v>
+      </c>
+      <c r="N48" s="8">
+        <v>8.8812895078046305E-3</v>
+      </c>
+      <c r="P48">
+        <v>40</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>8.4963423314003902E-3</v>
+      </c>
+      <c r="R48" s="9">
+        <v>8.2324211937105998E-3</v>
+      </c>
+      <c r="S48" s="8">
+        <v>9.1506899125305304E-3</v>
+      </c>
+      <c r="U48">
+        <v>40</v>
+      </c>
+      <c r="V48" s="8">
+        <v>8.5459137248501803E-3</v>
+      </c>
+      <c r="W48" s="8">
+        <v>8.7691243230960496E-3</v>
+      </c>
+      <c r="X48" s="9">
+        <v>8.5714114187602098E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>40</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="5">
         <v>97.442999999999998</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="6">
         <v>7.3817209430624897E-3</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="5">
         <v>162.339</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="6">
         <v>9.3784295212791004E-3</v>
       </c>
       <c r="G49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>21.290436460456384</v>
       </c>
       <c r="H49">
         <f>C49-E49</f>
         <v>-64.896000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <v>30</v>
+      </c>
+      <c r="L49" s="9">
+        <v>6.6941576862060998E-3</v>
+      </c>
+      <c r="M49" s="8">
+        <v>6.9116603769115003E-3</v>
+      </c>
+      <c r="N49" s="8">
+        <v>9.7760400279071295E-3</v>
+      </c>
+      <c r="P49">
+        <v>30</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>6.8556121357344303E-3</v>
+      </c>
+      <c r="R49" s="9">
+        <v>6.7432186711176602E-3</v>
+      </c>
+      <c r="S49" s="8">
+        <v>9.7113738124801098E-3</v>
+      </c>
+      <c r="U49">
+        <v>30</v>
+      </c>
+      <c r="V49" s="8">
+        <v>1.04523618121349E-2</v>
+      </c>
+      <c r="W49" s="8">
+        <v>1.04354849570336E-2</v>
+      </c>
+      <c r="X49" s="9">
+        <v>7.1158520942230102E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>30</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="5">
         <v>91.028000000000006</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="6">
         <v>8.2000667283049604E-3</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="5">
         <v>165.98500000000001</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="6">
         <v>1.0887481363737199E-2</v>
       </c>
       <c r="G50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>24.683529143693214</v>
       </c>
       <c r="H50">
         <f>C50-E50</f>
         <v>-74.957000000000008</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>20</v>
+      </c>
+      <c r="L50" s="9">
+        <v>5.0629683224929396E-3</v>
+      </c>
+      <c r="M50" s="8">
+        <v>4.9311083028856202E-3</v>
+      </c>
+      <c r="N50" s="8">
+        <v>5.7143648703596199E-3</v>
+      </c>
+      <c r="P50">
+        <v>20</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>5.1186210590626101E-3</v>
+      </c>
+      <c r="R50" s="9">
+        <v>4.8734342518153197E-3</v>
+      </c>
+      <c r="S50" s="8">
+        <v>6.0394199434187102E-3</v>
+      </c>
+      <c r="U50">
+        <v>20</v>
+      </c>
+      <c r="V50" s="8">
+        <v>5.5664670533434601E-3</v>
+      </c>
+      <c r="W50" s="8">
+        <v>5.73893272091224E-3</v>
+      </c>
+      <c r="X50" s="9">
+        <v>5.2156767436932596E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>20</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="5">
         <v>104.61</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="6">
         <v>7.0865690677605802E-3</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="5">
         <v>173.184</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="6">
         <v>8.4986582616171993E-3</v>
       </c>
       <c r="G51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>16.615436818233874</v>
       </c>
       <c r="H51">
         <f>C51-E51</f>
         <v>-68.573999999999998</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <v>10</v>
+      </c>
+      <c r="L51" s="9">
+        <v>1.92906768533565E-3</v>
+      </c>
+      <c r="M51" s="8">
+        <v>2.0817117098345002E-3</v>
+      </c>
+      <c r="N51" s="8">
+        <v>3.38690638055506E-3</v>
+      </c>
+      <c r="P51">
+        <v>10</v>
+      </c>
+      <c r="Q51" s="8">
+        <v>1.9922064506152099E-3</v>
+      </c>
+      <c r="R51" s="9">
+        <v>1.8482099486615501E-3</v>
+      </c>
+      <c r="S51" s="8">
+        <v>3.7056282054836998E-3</v>
+      </c>
+      <c r="U51">
+        <v>10</v>
+      </c>
+      <c r="V51" s="8">
+        <v>3.1530034311221199E-3</v>
+      </c>
+      <c r="W51" s="8">
+        <v>3.6413723005132999E-3</v>
+      </c>
+      <c r="X51" s="9">
+        <v>1.69901107564066E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B52">
         <v>10</v>
       </c>
-      <c r="G52" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C52" s="5">
+        <v>73.117999999999995</v>
+      </c>
+      <c r="D52" s="6">
+        <v>4.57732472301351E-3</v>
+      </c>
+      <c r="E52" s="5">
+        <v>185.048</v>
+      </c>
+      <c r="F52" s="6">
+        <v>7.2409690298524797E-3</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="8"/>
+        <v>36.785743674051261</v>
       </c>
       <c r="H52">
         <f>C52-E52</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+        <v>-111.93</v>
+      </c>
+      <c r="L52">
+        <f>AVERAGE(L42:L51)</f>
+        <v>5.7390325306030648E-3</v>
+      </c>
+      <c r="M52">
+        <f t="shared" ref="M52" si="9">AVERAGE(M42:M51)</f>
+        <v>6.4193799610480148E-3</v>
+      </c>
+      <c r="N52">
+        <f t="shared" ref="N52" si="10">AVERAGE(N42:N51)</f>
+        <v>7.9101710340164447E-3</v>
+      </c>
+      <c r="Q52">
+        <f>AVERAGE(Q42:Q51)</f>
+        <v>6.1179681099143837E-3</v>
+      </c>
+      <c r="R52">
+        <f t="shared" ref="R52" si="11">AVERAGE(R42:R51)</f>
+        <v>6.0714665456131104E-3</v>
+      </c>
+      <c r="S52">
+        <f t="shared" ref="S52" si="12">AVERAGE(S42:S51)</f>
+        <v>7.6350990995522269E-3</v>
+      </c>
+      <c r="V52">
+        <f>AVERAGE(V42:V51)</f>
+        <v>7.5052852324775723E-3</v>
+      </c>
+      <c r="W52">
+        <f t="shared" ref="W52" si="13">AVERAGE(W42:W51)</f>
+        <v>7.4700534999010432E-3</v>
+      </c>
+      <c r="X52">
+        <f t="shared" ref="X52" si="14">AVERAGE(X42:X51)</f>
+        <v>6.3571578760097487E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G53" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="L53" s="11"/>
+      <c r="M53" s="11">
+        <f>(M52-L52)/M52</f>
+        <v>0.10598335580277413</v>
+      </c>
+      <c r="N53" s="11">
+        <f>(N52-L52)/N52</f>
+        <v>0.27447428052778389</v>
+      </c>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11">
+        <f>(Q52-R52)/Q52</f>
+        <v>7.6008183543676573E-3</v>
+      </c>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11">
+        <f>(S52-R52)/S52</f>
+        <v>0.2047953187707568</v>
+      </c>
+      <c r="T53" s="11"/>
+      <c r="U53" s="11"/>
+      <c r="V53" s="11">
+        <f>(V52-X52)/V52</f>
+        <v>0.15297584580790341</v>
+      </c>
+      <c r="W53" s="11">
+        <f>(W52-X52)/W52</f>
+        <v>0.14898094423367078</v>
+      </c>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E54">
         <f>AVERAGE(E43:E52)</f>
-        <v>186.30899999999997</v>
+        <v>186.18289999999996</v>
       </c>
       <c r="G54" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H54">
         <f>AVERAGE(H43:H52)</f>
-        <v>-77.853099999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+        <v>-89.046099999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E55">
         <f>H54/E54</f>
-        <v>-0.41787084896596521</v>
+        <v>-0.47827217214899981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimisation for 2RC & param sweep set up
</commit_message>
<xml_diff>
--- a/PIECM/data/ECM_Params.xlsx
+++ b/PIECM/data/ECM_Params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katielukow/Documents/git-repos/PressureFitted_ECM/PIECM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549CCBED-966E-FC40-A8A8-78E60876E234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB421804-0DBF-4449-B095-7B85B6984BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15980" activeTab="1" xr2:uid="{35A3DEA1-7664-804A-B334-72214D1BA623}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15800" activeTab="1" xr2:uid="{35A3DEA1-7664-804A-B334-72214D1BA623}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>R1</t>
   </si>
@@ -119,14 +119,20 @@
   <si>
     <t>bad pressure fitting</t>
   </si>
+  <si>
+    <t>Mem</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -200,21 +206,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1895,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A2237-5B84-F146-A072-74BEF976396E}">
-  <dimension ref="B3:X55"/>
+  <dimension ref="B3:X66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J19" zoomScale="65" workbookViewId="0">
-      <selection activeCell="P60" sqref="P60"/>
+      <selection activeCell="P66" sqref="P66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1908,22 +1912,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C4">
@@ -2234,13 +2230,13 @@
       </c>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="K23" s="7">
+      <c r="K23" s="5">
         <v>40</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="5">
         <v>25</v>
       </c>
-      <c r="U23" s="7">
+      <c r="U23" s="5">
         <v>130</v>
       </c>
     </row>
@@ -2248,32 +2244,32 @@
       <c r="C24">
         <v>50</v>
       </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="9">
+      <c r="K24" s="6"/>
+      <c r="L24" s="7">
         <v>40</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M24" s="6">
         <v>25</v>
       </c>
-      <c r="N24" s="8">
+      <c r="N24" s="6">
         <v>130</v>
       </c>
-      <c r="Q24" s="8">
+      <c r="Q24" s="6">
         <v>40</v>
       </c>
-      <c r="R24" s="9">
+      <c r="R24" s="7">
         <v>25</v>
       </c>
-      <c r="S24" s="8">
+      <c r="S24" s="6">
         <v>130</v>
       </c>
-      <c r="V24" s="8">
+      <c r="V24" s="6">
         <v>40</v>
       </c>
-      <c r="W24" s="10">
+      <c r="W24" s="6">
         <v>25</v>
       </c>
-      <c r="X24" s="9">
+      <c r="X24" s="7">
         <v>130</v>
       </c>
     </row>
@@ -2284,10 +2280,10 @@
       <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G25" t="s">
@@ -2296,40 +2292,40 @@
       <c r="H25" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="6">
         <v>100</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="7">
         <v>1.20514085797111E-2</v>
       </c>
-      <c r="M25" s="8">
+      <c r="M25" s="6">
         <v>1.9713030785961299E-2</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="6">
         <v>2.1029734328836699E-2</v>
       </c>
       <c r="P25">
         <v>100</v>
       </c>
-      <c r="Q25" s="8">
+      <c r="Q25" s="6">
         <v>1.59337906151986E-2</v>
       </c>
-      <c r="R25" s="9">
+      <c r="R25" s="7">
         <v>1.0553681203737101E-2</v>
       </c>
-      <c r="S25" s="8">
+      <c r="S25" s="6">
         <v>1.01890979711316E-2</v>
       </c>
       <c r="U25">
         <v>100</v>
       </c>
-      <c r="V25" s="8">
+      <c r="V25" s="6">
         <v>1.8633937966488899E-2</v>
       </c>
-      <c r="W25" s="10">
+      <c r="W25" s="6">
         <v>1.1671043011221301E-2</v>
       </c>
-      <c r="X25" s="9">
+      <c r="X25" s="7">
         <v>8.4746770776052693E-3</v>
       </c>
     </row>
@@ -2337,16 +2333,16 @@
       <c r="B26">
         <v>100</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="3">
         <v>123.36499999999999</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>1.8482066102096901E-3</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="3">
         <v>106.42700000000001</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="4">
         <v>1.8482099486615501E-3</v>
       </c>
       <c r="G26">
@@ -2354,43 +2350,43 @@
         <v>1.8063163562275172E-4</v>
       </c>
       <c r="H26">
-        <f>C26-E26</f>
+        <f t="shared" ref="H26:H35" si="2">C26-E26</f>
         <v>16.937999999999988</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="6">
         <v>90</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="7">
         <v>1.38047882636651E-2</v>
       </c>
-      <c r="M26" s="8">
+      <c r="M26" s="6">
         <v>2.18504498144521E-2</v>
       </c>
-      <c r="N26" s="8">
+      <c r="N26" s="6">
         <v>2.5072392735572401E-2</v>
       </c>
       <c r="P26">
         <v>90</v>
       </c>
-      <c r="Q26" s="8">
+      <c r="Q26" s="6">
         <v>2.2670969303926699E-2</v>
       </c>
-      <c r="R26" s="9">
+      <c r="R26" s="7">
         <v>1.27019995049117E-2</v>
       </c>
-      <c r="S26" s="8">
+      <c r="S26" s="6">
         <v>1.3624210229426699E-2</v>
       </c>
       <c r="U26">
         <v>90</v>
       </c>
-      <c r="V26" s="8">
+      <c r="V26" s="6">
         <v>2.58659124799E-2</v>
       </c>
-      <c r="W26" s="10">
+      <c r="W26" s="6">
         <v>1.37625873167617E-2</v>
       </c>
-      <c r="X26" s="9">
+      <c r="X26" s="7">
         <v>1.2634663932254301E-2</v>
       </c>
     </row>
@@ -2398,60 +2394,60 @@
       <c r="B27">
         <v>90</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="3">
         <v>108.143</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="4">
         <v>4.8734322265080697E-3</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="3">
         <v>91.256</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="4">
         <v>4.8734342518153197E-3</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="G27:G35" si="2">(((F27-D27)/F27))*100</f>
+        <f t="shared" ref="G27:G35" si="3">(((F27-D27)/F27))*100</f>
         <v>4.1558111700784301E-5</v>
       </c>
       <c r="H27">
-        <f>C27-E27</f>
+        <f t="shared" si="2"/>
         <v>16.887</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="6">
         <v>80</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="7">
         <v>1.41096701366989E-2</v>
       </c>
-      <c r="M27" s="8">
+      <c r="M27" s="6">
         <v>2.2288955715876801E-2</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N27" s="6">
         <v>2.47730237027417E-2</v>
       </c>
       <c r="P27">
         <v>80</v>
       </c>
-      <c r="Q27" s="8">
+      <c r="Q27" s="6">
         <v>2.31406506107983E-2</v>
       </c>
-      <c r="R27" s="9">
+      <c r="R27" s="7">
         <v>1.2723955854867E-2</v>
       </c>
-      <c r="S27" s="8">
+      <c r="S27" s="6">
         <v>1.2884792524791199E-2</v>
       </c>
       <c r="U27">
         <v>80</v>
       </c>
-      <c r="V27" s="8">
+      <c r="V27" s="6">
         <v>2.5644508925281102E-2</v>
       </c>
-      <c r="W27" s="10">
+      <c r="W27" s="6">
         <v>1.3097780203017099E-2</v>
       </c>
-      <c r="X27" s="9">
+      <c r="X27" s="7">
         <v>1.25030175442527E-2</v>
       </c>
     </row>
@@ -2459,60 +2455,60 @@
       <c r="B28">
         <v>80</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="3">
         <v>109.63</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>6.74321854155402E-3</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="3">
         <v>93.792000000000002</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="4">
         <v>6.7432238681517697E-3</v>
       </c>
       <c r="G28">
+        <f t="shared" si="3"/>
+        <v>7.8991856919366645E-5</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="2"/>
-        <v>7.8991856919366645E-5</v>
-      </c>
-      <c r="H28">
-        <f>C28-E28</f>
         <v>15.837999999999994</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28" s="6">
         <v>70</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="7">
         <v>1.32266543475794E-2</v>
       </c>
-      <c r="M28" s="8">
+      <c r="M28" s="6">
         <v>2.2670899157301E-2</v>
       </c>
-      <c r="N28" s="8">
+      <c r="N28" s="6">
         <v>2.5615629651356601E-2</v>
       </c>
       <c r="P28">
         <v>70</v>
       </c>
-      <c r="Q28" s="8">
+      <c r="Q28" s="6">
         <v>2.3583449079185199E-2</v>
       </c>
-      <c r="R28" s="9">
+      <c r="R28" s="7">
         <v>1.1491399824413899E-2</v>
       </c>
-      <c r="S28" s="8">
+      <c r="S28" s="6">
         <v>1.2099811767114501E-2</v>
       </c>
       <c r="U28">
         <v>70</v>
       </c>
-      <c r="V28" s="8">
+      <c r="V28" s="6">
         <v>2.6560441229832199E-2</v>
       </c>
-      <c r="W28" s="10">
+      <c r="W28" s="6">
         <v>1.2345561977964501E-2</v>
       </c>
-      <c r="X28" s="9">
+      <c r="X28" s="7">
         <v>1.12878727291667E-2</v>
       </c>
     </row>
@@ -2520,60 +2516,60 @@
       <c r="B29">
         <v>70</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="3">
         <v>107.524</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>8.2324176714451101E-3</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="3">
         <v>91.650999999999996</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="4">
         <v>8.2324211937105998E-3</v>
       </c>
       <c r="G29">
+        <f t="shared" si="3"/>
+        <v>4.2785292525879602E-5</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="2"/>
-        <v>4.2785292525879602E-5</v>
-      </c>
-      <c r="H29">
-        <f>C29-E29</f>
         <v>15.873000000000005</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="6">
         <v>60</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="7">
         <v>1.21836701340103E-2</v>
       </c>
-      <c r="M29" s="8">
+      <c r="M29" s="6">
         <v>2.81357804840691E-2</v>
       </c>
-      <c r="N29" s="8">
+      <c r="N29" s="6">
         <v>3.06671418001358E-2</v>
       </c>
       <c r="P29">
         <v>60</v>
       </c>
-      <c r="Q29" s="8">
+      <c r="Q29" s="6">
         <v>2.7159823411525501E-2</v>
       </c>
-      <c r="R29" s="9">
+      <c r="R29" s="7">
         <v>1.08553110727237E-2</v>
       </c>
-      <c r="S29" s="8">
+      <c r="S29" s="6">
         <v>1.12826347218051E-2</v>
       </c>
       <c r="U29">
         <v>60</v>
       </c>
-      <c r="V29" s="8">
+      <c r="V29" s="6">
         <v>2.9995952555619199E-2</v>
       </c>
-      <c r="W29" s="10">
+      <c r="W29" s="6">
         <v>1.16594659287716E-2</v>
       </c>
-      <c r="X29" s="9">
+      <c r="X29" s="7">
         <v>1.0454981990813499E-2</v>
       </c>
     </row>
@@ -2581,60 +2577,60 @@
       <c r="B30">
         <v>60</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="3">
         <v>115.658</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>6.12830880190934E-3</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="3">
         <v>97.551000000000002</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="4">
         <v>6.1283105814866198E-3</v>
       </c>
       <c r="G30">
+        <f t="shared" si="3"/>
+        <v>2.9038627467473418E-5</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="2"/>
-        <v>2.9038627467473418E-5</v>
-      </c>
-      <c r="H30">
-        <f>C30-E30</f>
         <v>18.106999999999999</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30" s="6">
         <v>50</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="7">
         <v>1.2659332468500199E-2</v>
       </c>
-      <c r="M30" s="8">
+      <c r="M30" s="6">
         <v>2.43902848924837E-2</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N30" s="6">
         <v>2.8697577737195799E-2</v>
       </c>
       <c r="P30">
         <v>50</v>
       </c>
-      <c r="Q30" s="8">
+      <c r="Q30" s="6">
         <v>2.4963191054986698E-2</v>
       </c>
-      <c r="R30" s="9">
+      <c r="R30" s="7">
         <v>1.14578105002599E-2</v>
       </c>
-      <c r="S30" s="8">
+      <c r="S30" s="6">
         <v>1.24232275944178E-2</v>
       </c>
       <c r="U30">
         <v>50</v>
       </c>
-      <c r="V30" s="8">
+      <c r="V30" s="6">
         <v>2.9406206765896E-2</v>
       </c>
-      <c r="W30" s="10">
+      <c r="W30" s="6">
         <v>1.2896854003193301E-2</v>
       </c>
-      <c r="X30" s="9">
+      <c r="X30" s="7">
         <v>1.09311099701503E-2</v>
       </c>
     </row>
@@ -2642,60 +2638,60 @@
       <c r="B31">
         <v>50</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="3">
         <v>122.533</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <v>5.6433811165398102E-3</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="3">
         <v>104.126</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="4">
         <v>5.6433841006573301E-3</v>
       </c>
       <c r="G31">
+        <f t="shared" si="3"/>
+        <v>5.2878157267042065E-5</v>
+      </c>
+      <c r="H31">
         <f t="shared" si="2"/>
-        <v>5.2878157267042065E-5</v>
-      </c>
-      <c r="H31">
-        <f>C31-E31</f>
         <v>18.406999999999996</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31" s="6">
         <v>40</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="7">
         <v>1.2669031947247E-2</v>
       </c>
-      <c r="M31" s="8">
+      <c r="M31" s="6">
         <v>2.7015616999305998E-2</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="6">
         <v>3.1912495734792698E-2</v>
       </c>
       <c r="P31">
         <v>40</v>
       </c>
-      <c r="Q31" s="8">
+      <c r="Q31" s="6">
         <v>2.78957473928436E-2</v>
       </c>
-      <c r="R31" s="9">
+      <c r="R31" s="7">
         <v>1.05665027969922E-2</v>
       </c>
-      <c r="S31" s="8">
+      <c r="S31" s="6">
         <v>1.1651708213939699E-2</v>
       </c>
       <c r="U31">
         <v>40</v>
       </c>
-      <c r="V31" s="8">
+      <c r="V31" s="6">
         <v>3.2836644913086098E-2</v>
       </c>
-      <c r="W31" s="10">
+      <c r="W31" s="6">
         <v>1.2134285220434299E-2</v>
       </c>
-      <c r="X31" s="9">
+      <c r="X31" s="7">
         <v>9.9995181911557707E-3</v>
       </c>
     </row>
@@ -2703,60 +2699,60 @@
       <c r="B32">
         <v>40</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="3">
         <v>115.13</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="4">
         <v>7.3817190784420403E-3</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="3">
         <v>98.171000000000006</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="4">
         <v>7.3817209430624897E-3</v>
       </c>
       <c r="G32">
+        <f t="shared" si="3"/>
+        <v>2.5259969372252766E-5</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="2"/>
-        <v>2.5259969372252766E-5</v>
-      </c>
-      <c r="H32">
-        <f>C32-E32</f>
         <v>16.958999999999989</v>
       </c>
-      <c r="K32" s="8">
+      <c r="K32" s="6">
         <v>30</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="7">
         <v>1.2322098552017401E-2</v>
       </c>
-      <c r="M32" s="8">
+      <c r="M32" s="6">
         <v>3.2331230151346597E-2</v>
       </c>
-      <c r="N32" s="8">
+      <c r="N32" s="6">
         <v>3.76096003823033E-2</v>
       </c>
       <c r="P32">
         <v>30</v>
       </c>
-      <c r="Q32" s="8">
+      <c r="Q32" s="6">
         <v>3.3268453395697603E-2</v>
       </c>
-      <c r="R32" s="9">
+      <c r="R32" s="7">
         <v>9.5058096120956594E-3</v>
       </c>
-      <c r="S32" s="8">
+      <c r="S32" s="6">
         <v>1.0637769853062799E-2</v>
       </c>
       <c r="U32">
         <v>30</v>
       </c>
-      <c r="V32" s="8">
+      <c r="V32" s="6">
         <v>3.86100939532808E-2</v>
       </c>
-      <c r="W32" s="10">
+      <c r="W32" s="6">
         <v>1.13545033801898E-2</v>
       </c>
-      <c r="X32" s="9">
+      <c r="X32" s="7">
         <v>8.6455719579430195E-3</v>
       </c>
     </row>
@@ -2764,60 +2760,60 @@
       <c r="B33">
         <v>30</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="3">
         <v>107.619</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="4">
         <v>8.20006331598944E-3</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="3">
         <v>94.647999999999996</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="4">
         <v>8.2000667283049604E-3</v>
       </c>
       <c r="G33">
+        <f t="shared" si="3"/>
+        <v>4.1613265275572928E-5</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="2"/>
-        <v>4.1613265275572928E-5</v>
-      </c>
-      <c r="H33">
-        <f>C33-E33</f>
         <v>12.971000000000004</v>
       </c>
-      <c r="K33" s="8">
+      <c r="K33" s="6">
         <v>20</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33" s="7">
         <v>1.21388050928897E-2</v>
       </c>
-      <c r="M33" s="8">
+      <c r="M33" s="6">
         <v>3.8881886196302902E-2</v>
       </c>
-      <c r="N33" s="8">
+      <c r="N33" s="6">
         <v>4.3895324928647297E-2</v>
       </c>
       <c r="P33">
         <v>20</v>
       </c>
-      <c r="Q33" s="8">
+      <c r="Q33" s="6">
         <v>3.9535037684098197E-2</v>
       </c>
-      <c r="R33" s="9">
+      <c r="R33" s="7">
         <v>9.8111812025060904E-3</v>
       </c>
-      <c r="S33" s="8">
+      <c r="S33" s="6">
         <v>1.0399570112649701E-2</v>
       </c>
       <c r="U33">
         <v>20</v>
       </c>
-      <c r="V33" s="8">
+      <c r="V33" s="6">
         <v>4.47882721157234E-2</v>
       </c>
-      <c r="W33" s="10">
+      <c r="W33" s="6">
         <v>1.1687134651321599E-2</v>
       </c>
-      <c r="X33" s="9">
+      <c r="X33" s="7">
         <v>8.2208183093990302E-3</v>
       </c>
     </row>
@@ -2825,60 +2821,60 @@
       <c r="B34">
         <v>20</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="3">
         <v>120.7</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="4">
         <v>7.08656620464314E-3</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="3">
         <v>104.788</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="4">
         <v>7.08657574276725E-3</v>
       </c>
       <c r="G34">
+        <f t="shared" si="3"/>
+        <v>1.3459425900739919E-4</v>
+      </c>
+      <c r="H34">
         <f t="shared" si="2"/>
-        <v>1.3459425900739919E-4</v>
-      </c>
-      <c r="H34">
-        <f>C34-E34</f>
         <v>15.912000000000006</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34" s="6">
         <v>10</v>
       </c>
-      <c r="L34" s="9">
+      <c r="L34" s="7">
         <v>1.34770395067458E-2</v>
       </c>
-      <c r="M34" s="8">
+      <c r="M34" s="6">
         <v>4.3988460679129898E-2</v>
       </c>
-      <c r="N34" s="8">
+      <c r="N34" s="6">
         <v>4.93164375612654E-2</v>
       </c>
       <c r="P34">
         <v>10</v>
       </c>
-      <c r="Q34" s="8">
+      <c r="Q34" s="6">
         <v>4.5197875733679199E-2</v>
       </c>
-      <c r="R34" s="9">
+      <c r="R34" s="7">
         <v>1.2071505455972799E-2</v>
       </c>
-      <c r="S34" s="8">
+      <c r="S34" s="6">
         <v>1.30987175647654E-2</v>
       </c>
       <c r="U34">
         <v>10</v>
       </c>
-      <c r="V34" s="8">
+      <c r="V34" s="6">
         <v>5.0598526281017998E-2</v>
       </c>
-      <c r="W34" s="10">
+      <c r="W34" s="6">
         <v>1.3763290368036E-2</v>
       </c>
-      <c r="X34" s="9">
+      <c r="X34" s="7">
         <v>1.0485294217328901E-2</v>
       </c>
     </row>
@@ -2886,24 +2882,24 @@
       <c r="B35">
         <v>10</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="3">
         <v>85.790999999999997</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="4">
         <v>4.5773208474859601E-3</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="3">
         <v>74.596999999999994</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="4">
         <v>4.57732472301351E-3</v>
       </c>
       <c r="G35">
+        <f t="shared" si="3"/>
+        <v>8.4667961843208346E-5</v>
+      </c>
+      <c r="H35">
         <f t="shared" si="2"/>
-        <v>8.4667961843208346E-5</v>
-      </c>
-      <c r="H35">
-        <f>C35-E35</f>
         <v>11.194000000000003</v>
       </c>
       <c r="L35">
@@ -2911,11 +2907,11 @@
         <v>1.286424990290649E-2</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35" si="3">AVERAGE(M25:M34)</f>
+        <f t="shared" ref="M35" si="4">AVERAGE(M25:M34)</f>
         <v>2.812665948762294E-2</v>
       </c>
       <c r="N35">
-        <f t="shared" ref="N35" si="4">AVERAGE(N25:N34)</f>
+        <f t="shared" ref="N35" si="5">AVERAGE(N25:N34)</f>
         <v>3.185893585628477E-2</v>
       </c>
       <c r="Q35">
@@ -2923,11 +2919,11 @@
         <v>2.8334898828193962E-2</v>
       </c>
       <c r="R35">
-        <f t="shared" ref="R35" si="5">AVERAGE(R25:R34)</f>
+        <f t="shared" ref="R35" si="6">AVERAGE(R25:R34)</f>
         <v>1.1173915702848003E-2</v>
       </c>
       <c r="S35">
-        <f t="shared" ref="S35" si="6">AVERAGE(S25:S34)</f>
+        <f t="shared" ref="S35" si="7">AVERAGE(S25:S34)</f>
         <v>1.182915405531045E-2</v>
       </c>
       <c r="V35">
@@ -2935,11 +2931,11 @@
         <v>3.2294049718612571E-2</v>
       </c>
       <c r="W35">
-        <f t="shared" ref="W35:X35" si="7">AVERAGE(W25:W34)</f>
+        <f t="shared" ref="W35:X35" si="8">AVERAGE(W25:W34)</f>
         <v>1.243725060609112E-2</v>
       </c>
       <c r="X35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0363752592006949E-2</v>
       </c>
     </row>
@@ -2948,32 +2944,32 @@
         <f>AVERAGE(G26:G35)</f>
         <v>7.1201913700173097E-5</v>
       </c>
-      <c r="M36" s="11">
+      <c r="M36" s="8">
         <f>(M35-L35)/M35</f>
         <v>0.54263143447349771</v>
       </c>
-      <c r="N36" s="11">
+      <c r="N36" s="8">
         <f>(N35-L35)/N35</f>
         <v>0.5962121911121907</v>
       </c>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11">
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8">
         <f>(Q35-R35)/Q35</f>
         <v>0.60564829362546857</v>
       </c>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11">
+      <c r="R36" s="8"/>
+      <c r="S36" s="8">
         <f>(S35-R35)/S35</f>
         <v>5.5391818332798833E-2</v>
       </c>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11">
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8">
         <f>(V35-X35)/V35</f>
         <v>0.6790816672944604</v>
       </c>
-      <c r="W36" s="11">
+      <c r="W36" s="8">
         <f>(W35-X35)/W35</f>
         <v>0.1667167511337819</v>
       </c>
@@ -2999,13 +2995,13 @@
       </c>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="K40" s="7">
+      <c r="K40" s="5">
         <v>0</v>
       </c>
-      <c r="P40" s="7">
+      <c r="P40" s="5">
         <v>50</v>
       </c>
-      <c r="U40" s="7">
+      <c r="U40" s="5">
         <v>100</v>
       </c>
     </row>
@@ -3013,31 +3009,31 @@
       <c r="C41">
         <v>50</v>
       </c>
-      <c r="L41" s="9">
+      <c r="L41" s="7">
         <v>0</v>
       </c>
-      <c r="M41" s="8">
+      <c r="M41" s="6">
         <v>50</v>
       </c>
-      <c r="N41" s="8">
+      <c r="N41" s="6">
         <v>100</v>
       </c>
-      <c r="Q41" s="8">
+      <c r="Q41" s="6">
         <v>0</v>
       </c>
-      <c r="R41" s="9">
+      <c r="R41" s="7">
         <v>50</v>
       </c>
-      <c r="S41" s="8">
+      <c r="S41" s="6">
         <v>100</v>
       </c>
-      <c r="V41" s="8">
+      <c r="V41" s="6">
         <v>0</v>
       </c>
-      <c r="W41" s="8">
+      <c r="W41" s="6">
         <v>50</v>
       </c>
-      <c r="X41" s="9">
+      <c r="X41" s="7">
         <v>100</v>
       </c>
     </row>
@@ -3048,10 +3044,10 @@
       <c r="D42" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G42" t="s">
@@ -3063,37 +3059,37 @@
       <c r="K42">
         <v>100</v>
       </c>
-      <c r="L42" s="9">
+      <c r="L42" s="7">
         <v>3.6042557358412302E-3</v>
       </c>
-      <c r="M42" s="8">
+      <c r="M42" s="6">
         <v>6.0168176869929597E-3</v>
       </c>
-      <c r="N42" s="8">
+      <c r="N42" s="6">
         <v>8.7981339510285004E-3</v>
       </c>
       <c r="P42">
         <v>100</v>
       </c>
-      <c r="Q42" s="8">
+      <c r="Q42" s="6">
         <v>5.33802945454103E-3</v>
       </c>
-      <c r="R42" s="9">
+      <c r="R42" s="7">
         <v>4.57732472301351E-3</v>
       </c>
-      <c r="S42" s="8">
+      <c r="S42" s="6">
         <v>6.6928662190404902E-3</v>
       </c>
       <c r="U42">
         <v>100</v>
       </c>
-      <c r="V42" s="8">
+      <c r="V42" s="6">
         <v>8.1327277709610808E-3</v>
       </c>
-      <c r="W42" s="8">
+      <c r="W42" s="6">
         <v>6.3655580984447102E-3</v>
       </c>
-      <c r="X42" s="9">
+      <c r="X42" s="7">
         <v>5.0175673205011496E-3</v>
       </c>
     </row>
@@ -3101,16 +3097,16 @@
       <c r="B43">
         <v>100</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="3">
         <v>109.746</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="4">
         <v>1.8482120769911399E-3</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="3">
         <v>227.09399999999999</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="4">
         <v>3.6092468767544698E-3</v>
       </c>
       <c r="G43">
@@ -3118,43 +3114,43 @@
         <v>48.792306536451143</v>
       </c>
       <c r="H43">
-        <f>C43-E43</f>
+        <f t="shared" ref="H43:H52" si="9">C43-E43</f>
         <v>-117.348</v>
       </c>
       <c r="K43">
         <v>90</v>
       </c>
-      <c r="L43" s="9">
+      <c r="L43" s="7">
         <v>6.1310102754400702E-3</v>
       </c>
-      <c r="M43" s="8">
+      <c r="M43" s="6">
         <v>7.9869551352521294E-3</v>
       </c>
-      <c r="N43" s="8">
+      <c r="N43" s="6">
         <v>9.4230423392597795E-3</v>
       </c>
       <c r="P43">
         <v>90</v>
       </c>
-      <c r="Q43" s="8">
+      <c r="Q43" s="6">
         <v>7.1242398539241502E-3</v>
       </c>
-      <c r="R43" s="9">
+      <c r="R43" s="7">
         <v>7.0865702113395703E-3</v>
       </c>
-      <c r="S43" s="8">
+      <c r="S43" s="6">
         <v>8.4561259597547098E-3</v>
       </c>
       <c r="U43">
         <v>90</v>
       </c>
-      <c r="V43" s="8">
+      <c r="V43" s="6">
         <v>8.5517869904965897E-3</v>
       </c>
-      <c r="W43" s="8">
+      <c r="W43" s="6">
         <v>8.3111890308680495E-3</v>
       </c>
-      <c r="X43" s="9">
+      <c r="X43" s="7">
         <v>7.3007551798421402E-3</v>
       </c>
     </row>
@@ -3162,60 +3158,60 @@
       <c r="B44">
         <v>90</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="3">
         <v>98.156000000000006</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="4">
         <v>4.8734342518153197E-3</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="3">
         <v>188.709</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="4">
         <v>6.3996866180350796E-3</v>
       </c>
       <c r="G44">
-        <f t="shared" ref="G44:G54" si="8">((((F44-D44)/F44)))*100</f>
+        <f t="shared" ref="G44:G54" si="10">((((F44-D44)/F44)))*100</f>
         <v>23.848861003890391</v>
       </c>
       <c r="H44">
-        <f>C44-E44</f>
+        <f t="shared" si="9"/>
         <v>-90.552999999999997</v>
       </c>
       <c r="K44">
         <v>80</v>
       </c>
-      <c r="L44" s="9">
+      <c r="L44" s="7">
         <v>8.0483296607342207E-3</v>
       </c>
-      <c r="M44" s="8">
+      <c r="M44" s="6">
         <v>8.4036024040301995E-3</v>
       </c>
-      <c r="N44" s="8">
+      <c r="N44" s="6">
         <v>9.5322741770186604E-3</v>
       </c>
       <c r="P44">
         <v>80</v>
       </c>
-      <c r="Q44" s="8">
+      <c r="Q44" s="6">
         <v>8.2427533543529899E-3</v>
       </c>
-      <c r="R44" s="9">
+      <c r="R44" s="7">
         <v>8.2000667283049604E-3</v>
       </c>
-      <c r="S44" s="8">
+      <c r="S44" s="6">
         <v>9.3308233454571701E-3</v>
       </c>
       <c r="U44">
         <v>80</v>
       </c>
-      <c r="V44" s="8">
+      <c r="V44" s="6">
         <v>9.2305382292011493E-3</v>
       </c>
-      <c r="W44" s="8">
+      <c r="W44" s="6">
         <v>9.1653850851593499E-3</v>
       </c>
-      <c r="X44" s="9">
+      <c r="X44" s="7">
         <v>8.3881670010002296E-3</v>
       </c>
     </row>
@@ -3223,60 +3219,60 @@
       <c r="B45">
         <v>80</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="3">
         <v>96.052000000000007</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="4">
         <v>6.7432186711176602E-3</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="3">
         <v>186.25</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="4">
         <v>8.7308604768602197E-3</v>
       </c>
       <c r="G45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22.765703460850087</v>
       </c>
       <c r="H45">
-        <f>C45-E45</f>
+        <f t="shared" si="9"/>
         <v>-90.197999999999993</v>
       </c>
       <c r="K45">
         <v>70</v>
       </c>
-      <c r="L45" s="9">
+      <c r="L45" s="7">
         <v>7.2324080785703803E-3</v>
       </c>
-      <c r="M45" s="8">
+      <c r="M45" s="6">
         <v>7.4681367064375103E-3</v>
       </c>
-      <c r="N45" s="8">
+      <c r="N45" s="6">
         <v>8.7860224731295695E-3</v>
       </c>
       <c r="P45">
         <v>70</v>
       </c>
-      <c r="Q45" s="8">
+      <c r="Q45" s="6">
         <v>7.3139733543262E-3</v>
       </c>
-      <c r="R45" s="9">
+      <c r="R45" s="7">
         <v>7.3817209430624897E-3</v>
       </c>
-      <c r="S45" s="8">
+      <c r="S45" s="6">
         <v>8.7796313240783904E-3</v>
       </c>
       <c r="U45">
         <v>70</v>
       </c>
-      <c r="V45" s="8">
+      <c r="V45" s="6">
         <v>8.4060017337264405E-3</v>
       </c>
-      <c r="W45" s="8">
+      <c r="W45" s="6">
         <v>8.5307761418924408E-3</v>
       </c>
-      <c r="X45" s="9">
+      <c r="X45" s="7">
         <v>7.6651452086227596E-3</v>
       </c>
     </row>
@@ -3284,24 +3280,24 @@
       <c r="B46">
         <v>70</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="3">
         <v>96.04</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="4">
         <v>8.2324211937105998E-3</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="3">
         <v>193.006</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="4">
         <v>1.12317956992713E-2</v>
       </c>
       <c r="G46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>26.704318577974977</v>
       </c>
       <c r="H46">
-        <f>C46-E46</f>
+        <f t="shared" si="9"/>
         <v>-96.965999999999994</v>
       </c>
       <c r="J46">
@@ -3311,37 +3307,37 @@
       <c r="K46">
         <v>60</v>
       </c>
-      <c r="L46" s="9">
+      <c r="L46" s="7">
         <v>5.2886081405464696E-3</v>
       </c>
-      <c r="M46" s="8">
+      <c r="M46" s="6">
         <v>5.6904363009969098E-3</v>
       </c>
-      <c r="N46" s="8">
+      <c r="N46" s="6">
         <v>7.6975679522066597E-3</v>
       </c>
       <c r="P46">
         <v>60</v>
       </c>
-      <c r="Q46" s="8">
+      <c r="Q46" s="6">
         <v>5.3378813137547098E-3</v>
       </c>
-      <c r="R46" s="9">
+      <c r="R46" s="7">
         <v>5.6433841006573301E-3</v>
       </c>
-      <c r="S46" s="8">
+      <c r="S46" s="6">
         <v>7.67367061912708E-3</v>
       </c>
       <c r="U46">
         <v>60</v>
       </c>
-      <c r="V46" s="8">
+      <c r="V46" s="6">
         <v>7.0280008174422298E-3</v>
       </c>
-      <c r="W46" s="8">
+      <c r="W46" s="6">
         <v>7.2647518254569301E-3</v>
       </c>
-      <c r="X46" s="9">
+      <c r="X46" s="7">
         <v>6.1072279224231203E-3</v>
       </c>
     </row>
@@ -3349,60 +3345,60 @@
       <c r="B47">
         <v>60</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="3">
         <v>101.922</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="4">
         <v>6.1283146844481199E-3</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="3">
         <v>204.54300000000001</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="4">
         <v>3.3389006283308098E-3</v>
       </c>
       <c r="G47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-83.542889310599207</v>
       </c>
       <c r="H47">
-        <f>C47-E47</f>
+        <f t="shared" si="9"/>
         <v>-102.62100000000001</v>
       </c>
       <c r="K47">
         <v>50</v>
       </c>
-      <c r="L47" s="9">
+      <c r="L47" s="7">
         <v>5.1827892207384398E-3</v>
       </c>
-      <c r="M47" s="8">
+      <c r="M47" s="6">
         <v>6.2596898210953997E-3</v>
       </c>
-      <c r="N47" s="8">
+      <c r="N47" s="6">
         <v>7.1060686608948398E-3</v>
       </c>
       <c r="P47">
         <v>50</v>
       </c>
-      <c r="Q47" s="8">
+      <c r="Q47" s="6">
         <v>5.3600217914321104E-3</v>
       </c>
-      <c r="R47" s="9">
+      <c r="R47" s="7">
         <v>6.1283146844481199E-3</v>
       </c>
-      <c r="S47" s="8">
+      <c r="S47" s="6">
         <v>6.81076165415138E-3</v>
       </c>
       <c r="U47">
         <v>50</v>
       </c>
-      <c r="V47" s="8">
+      <c r="V47" s="6">
         <v>5.9860507614975696E-3</v>
       </c>
-      <c r="W47" s="8">
+      <c r="W47" s="6">
         <v>6.4779605156337697E-3</v>
       </c>
-      <c r="X47" s="9">
+      <c r="X47" s="7">
         <v>6.4907647953909497E-3</v>
       </c>
     </row>
@@ -3410,60 +3406,60 @@
       <c r="B48">
         <v>50</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="3">
         <v>103.253</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="4">
         <v>5.6433841006573301E-3</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="3">
         <v>175.67099999999999</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="4">
         <v>6.7769888148821698E-3</v>
       </c>
       <c r="G48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>16.727262582099296</v>
       </c>
       <c r="H48">
-        <f>C48-E48</f>
+        <f t="shared" si="9"/>
         <v>-72.417999999999992</v>
       </c>
       <c r="K48">
         <v>40</v>
       </c>
-      <c r="L48" s="9">
+      <c r="L48" s="7">
         <v>8.2167305001251394E-3</v>
       </c>
-      <c r="M48" s="8">
+      <c r="M48" s="6">
         <v>8.4436811660434201E-3</v>
       </c>
-      <c r="N48" s="8">
+      <c r="N48" s="6">
         <v>8.8812895078046305E-3</v>
       </c>
       <c r="P48">
         <v>40</v>
       </c>
-      <c r="Q48" s="8">
+      <c r="Q48" s="6">
         <v>8.4963423314003902E-3</v>
       </c>
-      <c r="R48" s="9">
+      <c r="R48" s="7">
         <v>8.2324211937105998E-3</v>
       </c>
-      <c r="S48" s="8">
+      <c r="S48" s="6">
         <v>9.1506899125305304E-3</v>
       </c>
       <c r="U48">
         <v>40</v>
       </c>
-      <c r="V48" s="8">
+      <c r="V48" s="6">
         <v>8.5459137248501803E-3</v>
       </c>
-      <c r="W48" s="8">
+      <c r="W48" s="6">
         <v>8.7691243230960496E-3</v>
       </c>
-      <c r="X48" s="9">
+      <c r="X48" s="7">
         <v>8.5714114187602098E-3</v>
       </c>
     </row>
@@ -3471,60 +3467,60 @@
       <c r="B49">
         <v>40</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="3">
         <v>97.442999999999998</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="4">
         <v>7.3817209430624897E-3</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="3">
         <v>162.339</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="4">
         <v>9.3784295212791004E-3</v>
       </c>
       <c r="G49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.290436460456384</v>
       </c>
       <c r="H49">
-        <f>C49-E49</f>
+        <f t="shared" si="9"/>
         <v>-64.896000000000001</v>
       </c>
       <c r="K49">
         <v>30</v>
       </c>
-      <c r="L49" s="9">
+      <c r="L49" s="7">
         <v>6.6941576862060998E-3</v>
       </c>
-      <c r="M49" s="8">
+      <c r="M49" s="6">
         <v>6.9116603769115003E-3</v>
       </c>
-      <c r="N49" s="8">
+      <c r="N49" s="6">
         <v>9.7760400279071295E-3</v>
       </c>
       <c r="P49">
         <v>30</v>
       </c>
-      <c r="Q49" s="8">
+      <c r="Q49" s="6">
         <v>6.8556121357344303E-3</v>
       </c>
-      <c r="R49" s="9">
+      <c r="R49" s="7">
         <v>6.7432186711176602E-3</v>
       </c>
-      <c r="S49" s="8">
+      <c r="S49" s="6">
         <v>9.7113738124801098E-3</v>
       </c>
       <c r="U49">
         <v>30</v>
       </c>
-      <c r="V49" s="8">
+      <c r="V49" s="6">
         <v>1.04523618121349E-2</v>
       </c>
-      <c r="W49" s="8">
+      <c r="W49" s="6">
         <v>1.04354849570336E-2</v>
       </c>
-      <c r="X49" s="9">
+      <c r="X49" s="7">
         <v>7.1158520942230102E-3</v>
       </c>
     </row>
@@ -3532,60 +3528,60 @@
       <c r="B50">
         <v>30</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="3">
         <v>91.028000000000006</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="4">
         <v>8.2000667283049604E-3</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="3">
         <v>165.98500000000001</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="4">
         <v>1.0887481363737199E-2</v>
       </c>
       <c r="G50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>24.683529143693214</v>
       </c>
       <c r="H50">
-        <f>C50-E50</f>
+        <f t="shared" si="9"/>
         <v>-74.957000000000008</v>
       </c>
       <c r="K50">
         <v>20</v>
       </c>
-      <c r="L50" s="9">
+      <c r="L50" s="7">
         <v>5.0629683224929396E-3</v>
       </c>
-      <c r="M50" s="8">
+      <c r="M50" s="6">
         <v>4.9311083028856202E-3</v>
       </c>
-      <c r="N50" s="8">
+      <c r="N50" s="6">
         <v>5.7143648703596199E-3</v>
       </c>
       <c r="P50">
         <v>20</v>
       </c>
-      <c r="Q50" s="8">
+      <c r="Q50" s="6">
         <v>5.1186210590626101E-3</v>
       </c>
-      <c r="R50" s="9">
+      <c r="R50" s="7">
         <v>4.8734342518153197E-3</v>
       </c>
-      <c r="S50" s="8">
+      <c r="S50" s="6">
         <v>6.0394199434187102E-3</v>
       </c>
       <c r="U50">
         <v>20</v>
       </c>
-      <c r="V50" s="8">
+      <c r="V50" s="6">
         <v>5.5664670533434601E-3</v>
       </c>
-      <c r="W50" s="8">
+      <c r="W50" s="6">
         <v>5.73893272091224E-3</v>
       </c>
-      <c r="X50" s="9">
+      <c r="X50" s="7">
         <v>5.2156767436932596E-3</v>
       </c>
     </row>
@@ -3593,60 +3589,60 @@
       <c r="B51">
         <v>20</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="3">
         <v>104.61</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="4">
         <v>7.0865690677605802E-3</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="3">
         <v>173.184</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51" s="4">
         <v>8.4986582616171993E-3</v>
       </c>
       <c r="G51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>16.615436818233874</v>
       </c>
       <c r="H51">
-        <f>C51-E51</f>
+        <f t="shared" si="9"/>
         <v>-68.573999999999998</v>
       </c>
       <c r="K51">
         <v>10</v>
       </c>
-      <c r="L51" s="9">
+      <c r="L51" s="7">
         <v>1.92906768533565E-3</v>
       </c>
-      <c r="M51" s="8">
+      <c r="M51" s="6">
         <v>2.0817117098345002E-3</v>
       </c>
-      <c r="N51" s="8">
+      <c r="N51" s="6">
         <v>3.38690638055506E-3</v>
       </c>
       <c r="P51">
         <v>10</v>
       </c>
-      <c r="Q51" s="8">
+      <c r="Q51" s="6">
         <v>1.9922064506152099E-3</v>
       </c>
-      <c r="R51" s="9">
+      <c r="R51" s="7">
         <v>1.8482099486615501E-3</v>
       </c>
-      <c r="S51" s="8">
+      <c r="S51" s="6">
         <v>3.7056282054836998E-3</v>
       </c>
       <c r="U51">
         <v>10</v>
       </c>
-      <c r="V51" s="8">
+      <c r="V51" s="6">
         <v>3.1530034311221199E-3</v>
       </c>
-      <c r="W51" s="8">
+      <c r="W51" s="6">
         <v>3.6413723005132999E-3</v>
       </c>
-      <c r="X51" s="9">
+      <c r="X51" s="7">
         <v>1.69901107564066E-3</v>
       </c>
     </row>
@@ -3654,24 +3650,24 @@
       <c r="B52">
         <v>10</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="3">
         <v>73.117999999999995</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="4">
         <v>4.57732472301351E-3</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="3">
         <v>185.048</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="4">
         <v>7.2409690298524797E-3</v>
       </c>
       <c r="G52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>36.785743674051261</v>
       </c>
       <c r="H52">
-        <f>C52-E52</f>
+        <f t="shared" si="9"/>
         <v>-111.93</v>
       </c>
       <c r="L52">
@@ -3679,11 +3675,11 @@
         <v>5.7390325306030648E-3</v>
       </c>
       <c r="M52">
-        <f t="shared" ref="M52" si="9">AVERAGE(M42:M51)</f>
+        <f t="shared" ref="M52" si="11">AVERAGE(M42:M51)</f>
         <v>6.4193799610480148E-3</v>
       </c>
       <c r="N52">
-        <f t="shared" ref="N52" si="10">AVERAGE(N42:N51)</f>
+        <f t="shared" ref="N52" si="12">AVERAGE(N42:N51)</f>
         <v>7.9101710340164447E-3</v>
       </c>
       <c r="Q52">
@@ -3691,11 +3687,11 @@
         <v>6.1179681099143837E-3</v>
       </c>
       <c r="R52">
-        <f t="shared" ref="R52" si="11">AVERAGE(R42:R51)</f>
+        <f t="shared" ref="R52" si="13">AVERAGE(R42:R51)</f>
         <v>6.0714665456131104E-3</v>
       </c>
       <c r="S52">
-        <f t="shared" ref="S52" si="12">AVERAGE(S42:S51)</f>
+        <f t="shared" ref="S52" si="14">AVERAGE(S42:S51)</f>
         <v>7.6350990995522269E-3</v>
       </c>
       <c r="V52">
@@ -3703,46 +3699,46 @@
         <v>7.5052852324775723E-3</v>
       </c>
       <c r="W52">
-        <f t="shared" ref="W52" si="13">AVERAGE(W42:W51)</f>
+        <f t="shared" ref="W52" si="15">AVERAGE(W42:W51)</f>
         <v>7.4700534999010432E-3</v>
       </c>
       <c r="X52">
-        <f t="shared" ref="X52" si="14">AVERAGE(X42:X51)</f>
+        <f t="shared" ref="X52" si="16">AVERAGE(X42:X51)</f>
         <v>6.3571578760097487E-3</v>
       </c>
     </row>
     <row r="53" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G53" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11">
+      <c r="L53" s="8"/>
+      <c r="M53" s="8">
         <f>(M52-L52)/M52</f>
         <v>0.10598335580277413</v>
       </c>
-      <c r="N53" s="11">
+      <c r="N53" s="8">
         <f>(N52-L52)/N52</f>
         <v>0.27447428052778389</v>
       </c>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11">
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8">
         <f>(Q52-R52)/Q52</f>
         <v>7.6008183543676573E-3</v>
       </c>
-      <c r="R53" s="11"/>
-      <c r="S53" s="11">
+      <c r="R53" s="8"/>
+      <c r="S53" s="8">
         <f>(S52-R52)/S52</f>
         <v>0.2047953187707568</v>
       </c>
-      <c r="T53" s="11"/>
-      <c r="U53" s="11"/>
-      <c r="V53" s="11">
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="8">
         <f>(V52-X52)/V52</f>
         <v>0.15297584580790341</v>
       </c>
-      <c r="W53" s="11">
+      <c r="W53" s="8">
         <f>(W52-X52)/W52</f>
         <v>0.14898094423367078</v>
       </c>
@@ -3753,7 +3749,7 @@
         <v>186.18289999999996</v>
       </c>
       <c r="G54" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H54">
@@ -3765,6 +3761,126 @@
       <c r="E55">
         <f>H54/E54</f>
         <v>-0.47827217214899981</v>
+      </c>
+    </row>
+    <row r="58" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>40</v>
+      </c>
+      <c r="M58">
+        <v>25</v>
+      </c>
+      <c r="N58">
+        <v>130</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>50</v>
+      </c>
+      <c r="R58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="K59" t="s">
+        <v>28</v>
+      </c>
+      <c r="L59">
+        <v>3.585</v>
+      </c>
+      <c r="M59">
+        <v>3.7229999999999999</v>
+      </c>
+      <c r="N59">
+        <v>3.67</v>
+      </c>
+      <c r="P59">
+        <v>4.4539999999999997</v>
+      </c>
+      <c r="Q59">
+        <v>3.956</v>
+      </c>
+      <c r="R59">
+        <v>3.8069999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="K60" t="s">
+        <v>27</v>
+      </c>
+      <c r="L60">
+        <v>2.94</v>
+      </c>
+      <c r="M60">
+        <v>3.08</v>
+      </c>
+      <c r="N60">
+        <v>2.97</v>
+      </c>
+      <c r="P60">
+        <v>3.4</v>
+      </c>
+      <c r="Q60">
+        <v>2.83</v>
+      </c>
+      <c r="R60">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="64" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="L64">
+        <v>40</v>
+      </c>
+      <c r="M64">
+        <v>25</v>
+      </c>
+      <c r="N64">
+        <v>130</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>50</v>
+      </c>
+      <c r="R64">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K65" t="s">
+        <v>28</v>
+      </c>
+      <c r="L65">
+        <v>7.976</v>
+      </c>
+      <c r="M65">
+        <v>9.16</v>
+      </c>
+      <c r="N65">
+        <v>8.6110000000000007</v>
+      </c>
+      <c r="P65">
+        <v>10.807</v>
+      </c>
+    </row>
+    <row r="66" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K66" t="s">
+        <v>27</v>
+      </c>
+      <c r="L66">
+        <v>5.97</v>
+      </c>
+      <c r="M66">
+        <v>5.55</v>
+      </c>
+      <c r="N66">
+        <v>5.42</v>
+      </c>
+      <c r="P66">
+        <v>4.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>